<commit_message>
update new URL 104.211.52.121
</commit_message>
<xml_diff>
--- a/TravelWithUs/TestData/Login.xlsx
+++ b/TravelWithUs/TestData/Login.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Framework\Protractor framework\Demo\TravelWithUs\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Framework\Protractor framework\Protractor_NonAngularJS\TravelWithUs\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -75,13 +75,13 @@
     <t>female</t>
   </si>
   <si>
-    <t>ptvanh5@mailinator.com</t>
-  </si>
-  <si>
     <t>TC02</t>
   </si>
   <si>
     <t>TC01</t>
+  </si>
+  <si>
+    <t>ptvanh10@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -427,7 +427,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -438,7 +438,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,7 +532,7 @@
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
update for dependent suites
</commit_message>
<xml_diff>
--- a/TravelWithUs/TestData/Login.xlsx
+++ b/TravelWithUs/TestData/Login.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>TestcaseID</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>ptvanh@mailinator.com</t>
-  </si>
-  <si>
     <t>invalidPassword</t>
   </si>
   <si>
@@ -81,7 +78,7 @@
     <t>TC01</t>
   </si>
   <si>
-    <t>ptvanh10@mailinator.com</t>
+    <t>ptvanh9@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -403,8 +400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,10 +424,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
       <c r="C2">
         <v>123456</v>
@@ -438,31 +435,31 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>123456</v>
@@ -478,7 +475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -497,45 +494,45 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G2">
         <v>123456</v>

</xml_diff>

<commit_message>
update on 23 Dec
</commit_message>
<xml_diff>
--- a/TravelWithUs/TestData/Login.xlsx
+++ b/TravelWithUs/TestData/Login.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>TestcaseID</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>ptvanh9@mailinator.com</t>
+  </si>
+  <si>
+    <t>ptvanh@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -401,7 +404,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +430,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>123456</v>
@@ -454,7 +457,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>